<commit_message>
remove spaces and руб.
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>url</t>
   </si>
@@ -38,43 +38,28 @@
     <t>https://www.nix.ru/autocatalog/server_systems_intel/Intel-2U-R2208WT2YSR-LGA2011-3-C612-2xPCI-E-SVGA-SATA-RAID-8xHotSwapSAS-SATA-2xGbLAN-24DDR4-1100W_280008.html</t>
   </si>
   <si>
-    <t>106 829 руб.</t>
-  </si>
-  <si>
     <t>✔Серверная платформа 2U ✔Socket LGA2011-3 Narrow ILM x2 ✔Цвет: Черный ✔Registered DDR4, LRDIMM DDR4 ✔8 корзин HotSwap 2.5" ✔2x 10 Гбит / с ✔IPMI (Intelligent Platform Management Interface)</t>
   </si>
   <si>
     <t>https://www.nix.ru/autocatalog/asus/asustek_video/11Gb-PCI-E-GDDR6-ASUS-DUAL-RTX2080TI-O11G-RTL-HDMI-plus-3xDP-plus-SLI-plus-USB-C-GeForce-RTX2080Ti_373803.html</t>
   </si>
   <si>
-    <t>103 475 руб.</t>
-  </si>
-  <si>
     <t>✔11 Гб ✔PCI Express 3.0 16x ✔GDDR6 ✔VR Ready ✔3 выхода DisplayPort, HDMI 2.0b, USB Type-C ✔Поддержка SLI ✔GeForce® RTX 2080 Ti ✔352 бита ✔Проприетарное охлаждение</t>
   </si>
   <si>
     <t>https://www.nix.ru/autocatalog/cases_exegate/Server-Case-4U-Exegate-Pro-4019S-ATX-600W-24-plus-8-plus-2x4-plus-2x6-8pin-EX244592RUS_293721.html</t>
   </si>
   <si>
-    <t>7 290 руб.</t>
-  </si>
-  <si>
     <t>Cерверный корпус 4U 600 Вт ✔2 вентилятора</t>
   </si>
   <si>
     <t>https://www.nix.ru/autocatalog/memory_modules_goodram/Goodram-IR-2400D464L15S-4G-DDR4-DIMM-4Gb-PC4-19200-CL15_319761.html</t>
   </si>
   <si>
-    <t>1 987 руб.</t>
-  </si>
-  <si>
     <t>✔4 Гб x 1 шт. ✔DDR4 ✔PC4-19200 (DDR4 2400 МГц) ✔до 2400 МГц ✔Радиатор</t>
   </si>
   <si>
     <t>https://www.nix.ru/autocatalog/modding/Akasa-AK-LD05-50GN-Vegas-M-Green-50sm-15LED-magnit_379368.html</t>
-  </si>
-  <si>
-    <t>910 руб.</t>
   </si>
   <si>
     <t>Светодиодная лента</t>
@@ -416,14 +401,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="1" width="158.015701293945" customWidth="1"/>
-    <col min="2" max="2" width="11.7275838851929" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="184.310531616211" customWidth="1"/>
   </cols>
   <sheetData>
@@ -442,62 +427,62 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="0">
+        <v>106829</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0">
+        <v>103475</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="0">
+        <v>7290</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="0">
+        <v>1987</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="0">
+        <v>910</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId11"/>
+    <hyperlink ref="A3" r:id="rId12"/>
+    <hyperlink ref="A4" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>